<commit_message>
Added a gantt chart and template for the final report
</commit_message>
<xml_diff>
--- a/gantt_chart.xlsx
+++ b/gantt_chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d1788031b08e836/Documents/Josh/University/Year 3/CM3203 - Individual Project/Identifying-Urban-Functional-Regions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{3343BC79-A2D5-4CCA-B22B-FBF7918A30EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25F3D708-5BCD-4DD6-8E87-7FD5069B88C7}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{3343BC79-A2D5-4CCA-B22B-FBF7918A30EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62DFB2F7-359B-4F45-8E2D-2EB0E80D4125}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2BCE16E2-705E-4E2B-A759-3BDCB34CE93F}"/>
+    <workbookView minimized="1" xWindow="-5688" yWindow="204" windowWidth="17280" windowHeight="8880" xr2:uid="{2BCE16E2-705E-4E2B-A759-3BDCB34CE93F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,6 +101,24 @@
     <t>Report</t>
   </si>
   <si>
+    <t xml:space="preserve">                    ☑</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               ☑ D</t>
+  </si>
+  <si>
+    <t>☑ = milestone     D = deliverable</t>
+  </si>
+  <si>
+    <t>Implementation - Correlation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         ☑ ☑ D </t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">           </t>
     </r>
@@ -112,41 +130,44 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">    </t>
+      <t xml:space="preserve">  </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
       </rPr>
       <t>☑ D</t>
     </r>
   </si>
-  <si>
-    <t xml:space="preserve">                    ☑</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               ☑ D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         ☑ D ☑</t>
-  </si>
-  <si>
-    <t>☑ = milestone     D = deliverable</t>
-  </si>
-  <si>
-    <t>Implementation - Correlation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               </t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,11 +197,19 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,6 +222,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CC00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1AE66D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -333,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -357,8 +398,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,6 +408,15 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF1AE66D"/>
+      <color rgb="FF19E71E"/>
+      <color rgb="FF10F025"/>
+      <color rgb="FF00FF00"/>
+      <color rgb="FF00CC00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -375,6 +426,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -696,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E25DE3-BD96-4466-B9EE-ADB655D59988}">
   <dimension ref="C3:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,7 +762,7 @@
   <sheetData>
     <row r="3" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C3" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>0</v>
@@ -751,8 +806,8 @@
       <c r="C4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>21</v>
+      <c r="D4" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="E4" s="1"/>
       <c r="O4" s="6"/>
@@ -761,8 +816,8 @@
       <c r="C5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>22</v>
+      <c r="E5" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="F5" s="1"/>
       <c r="O5" s="6"/>
@@ -772,10 +827,10 @@
         <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" s="1"/>
       <c r="O6" s="6"/>
@@ -785,7 +840,7 @@
         <v>15</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -796,10 +851,10 @@
         <v>16</v>
       </c>
       <c r="H8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -811,22 +866,20 @@
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L9" s="1"/>
       <c r="O9" s="6"/>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C10" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
+        <v>24</v>
+      </c>
       <c r="K10" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L10" s="1"/>
       <c r="O10" s="6"/>
@@ -836,7 +889,7 @@
         <v>18</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M11" s="1"/>
       <c r="O11" s="6"/>
@@ -847,7 +900,7 @@
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="7"/>
@@ -868,7 +921,7 @@
       <c r="M13" s="4"/>
       <c r="N13" s="5"/>
       <c r="O13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.3">

</xml_diff>